<commit_message>
Come back after a year.
</commit_message>
<xml_diff>
--- a/File/Excel.xlsx
+++ b/File/Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\Persian_Podcasts\File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22ACF091-A38F-49B8-860F-50F6BFB859F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4659CE3D-75E2-4BB4-B7AF-AC99B56172DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{FF410003-BA4E-4957-A6FD-127020229CB5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>شماره</t>
   </si>
@@ -42,13 +42,7 @@
     <t>اسم</t>
   </si>
   <si>
-    <t>نماد</t>
-  </si>
-  <si>
     <t>میزبان</t>
-  </si>
-  <si>
-    <t>لینک</t>
   </si>
   <si>
     <t>موضوع</t>
@@ -94,19 +88,10 @@
     </r>
   </si>
   <si>
-    <t>..\Logo\Music\Esm Nadareh.jpg</t>
-  </si>
-  <si>
-    <t>آخرین به‌روزرسانی اطلاعات</t>
-  </si>
-  <si>
-    <t>تاریخ آخرین قسمت منتشر شده</t>
-  </si>
-  <si>
-    <t>5 فروردین 1403</t>
-  </si>
-  <si>
     <t>YouTube Channel</t>
+  </si>
+  <si>
+    <t>کانال منتشرکننده</t>
   </si>
 </sst>
 </file>
@@ -221,7 +206,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -240,12 +225,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -565,20 +544,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B41373AA-59E7-4276-BA18-C69D11EC7714}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.7109375" defaultRowHeight="54.95" customHeight="1" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="55.7109375" style="2"/>
-    <col min="6" max="6" width="55.7109375" style="7"/>
-    <col min="7" max="16384" width="55.7109375" style="2"/>
+    <col min="1" max="16384" width="55.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="54.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="54.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -586,117 +563,101 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="54.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="54.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="54.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" ht="54.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="54.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="54.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="54.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:5" ht="54.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="54.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="54.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="54.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="54.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="54.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="54.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="54.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="54.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="54.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="54.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{0746AF53-0A63-4A95-B4E0-0524CDE3266F}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{140378A4-60BB-433E-A39C-7B7562CCD09A}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{140378A4-60BB-433E-A39C-7B7562CCD09A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId3"/>
+  <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>